<commit_message>
Change frailty shape (to segmented linear regression)
</commit_message>
<xml_diff>
--- a/data/frailty/chronic-diseases-canada.xlsx
+++ b/data/frailty/chronic-diseases-canada.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="32360" windowHeight="24100" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="2013" sheetId="2" r:id="rId1"/>
@@ -181,9 +181,6 @@
     <t>Data from 2013 &amp; 2014 report on chronic obstructive pulmonary disease only</t>
   </si>
   <si>
-    <t>Data from 2015 &amp;  2016 roport more broadly on chronic respiratory diseases</t>
-  </si>
-  <si>
     <t>prop_chronic</t>
   </si>
   <si>
@@ -191,6 +188,9 @@
   </si>
   <si>
     <t>arbitrary mult</t>
+  </si>
+  <si>
+    <t>Data from 2015 &amp;  2016 report more broadly on chronic respiratory diseases</t>
   </si>
 </sst>
 </file>
@@ -891,11 +891,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2144299096"/>
-        <c:axId val="-2140714824"/>
+        <c:axId val="2056007416"/>
+        <c:axId val="2056010536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2144299096"/>
+        <c:axId val="2056007416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -904,7 +904,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2140714824"/>
+        <c:crossAx val="2056010536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -912,7 +912,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2140714824"/>
+        <c:axId val="2056010536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -923,7 +923,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144299096"/>
+        <c:crossAx val="2056007416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1113,11 +1113,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2139745912"/>
-        <c:axId val="-2139735256"/>
+        <c:axId val="2056067544"/>
+        <c:axId val="2056073784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2139745912"/>
+        <c:axId val="2056067544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1127,12 +1127,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2139735256"/>
+        <c:crossAx val="2056073784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2139735256"/>
+        <c:axId val="2056073784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1143,7 +1143,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2139745912"/>
+        <c:crossAx val="2056067544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1328,11 +1328,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2145660424"/>
-        <c:axId val="-2144591704"/>
+        <c:axId val="2056105096"/>
+        <c:axId val="2056108056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2145660424"/>
+        <c:axId val="2056105096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1342,12 +1342,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144591704"/>
+        <c:crossAx val="2056108056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2144591704"/>
+        <c:axId val="2056108056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1359,7 +1359,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145660424"/>
+        <c:crossAx val="2056105096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2939,8 +2939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3227,7 +3227,7 @@
     </row>
     <row r="23" spans="2:7">
       <c r="B23" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -3238,7 +3238,7 @@
     <row r="26" spans="2:7" ht="16" thickBot="1"/>
     <row r="27" spans="2:7" ht="16" thickBot="1">
       <c r="E27" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F27" s="6">
         <v>1.5</v>
@@ -3246,16 +3246,16 @@
     </row>
     <row r="29" spans="2:7">
       <c r="C29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="2:7">
       <c r="B30" s="3">
-        <f t="shared" ref="B30:B33" si="0">B31-5</f>
+        <f t="shared" ref="B30:B32" si="0">B31-5</f>
         <v>0</v>
       </c>
       <c r="C30" s="3">
@@ -3327,11 +3327,11 @@
     </row>
     <row r="34" spans="2:6">
       <c r="B34">
-        <f>LEFT(B4,2)*1</f>
+        <f t="shared" ref="B34:B46" si="4">LEFT(B4,2)*1</f>
         <v>20</v>
       </c>
       <c r="C34">
-        <f>F4/100</f>
+        <f t="shared" ref="C34:C46" si="5">F4/100</f>
         <v>0.11699999999999999</v>
       </c>
       <c r="E34" s="7">
@@ -3345,11 +3345,11 @@
     </row>
     <row r="35" spans="2:6">
       <c r="B35">
-        <f>LEFT(B5,2)*1</f>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="C35">
-        <f>F5/100</f>
+        <f t="shared" si="5"/>
         <v>0.115</v>
       </c>
       <c r="E35" s="7">
@@ -3363,11 +3363,11 @@
     </row>
     <row r="36" spans="2:6">
       <c r="B36">
-        <f>LEFT(B6,2)*1</f>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="C36">
-        <f>F6/100</f>
+        <f t="shared" si="5"/>
         <v>8.8000000000000009E-2</v>
       </c>
       <c r="E36" s="7">
@@ -3381,11 +3381,11 @@
     </row>
     <row r="37" spans="2:6">
       <c r="B37">
-        <f>LEFT(B7,2)*1</f>
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
       <c r="C37">
-        <f>F7/100</f>
+        <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
       <c r="E37" s="7">
@@ -3399,11 +3399,11 @@
     </row>
     <row r="38" spans="2:6">
       <c r="B38">
-        <f>LEFT(B8,2)*1</f>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="C38">
-        <f>F8/100</f>
+        <f t="shared" si="5"/>
         <v>0.125</v>
       </c>
       <c r="E38" s="7">
@@ -3417,11 +3417,11 @@
     </row>
     <row r="39" spans="2:6">
       <c r="B39">
-        <f>LEFT(B9,2)*1</f>
+        <f t="shared" si="4"/>
         <v>45</v>
       </c>
       <c r="C39">
-        <f>F9/100</f>
+        <f t="shared" si="5"/>
         <v>0.157</v>
       </c>
       <c r="E39" s="7">
@@ -3435,11 +3435,11 @@
     </row>
     <row r="40" spans="2:6">
       <c r="B40">
-        <f>LEFT(B10,2)*1</f>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="C40">
-        <f>F10/100</f>
+        <f t="shared" si="5"/>
         <v>0.20199999999999999</v>
       </c>
       <c r="E40" s="7">
@@ -3453,11 +3453,11 @@
     </row>
     <row r="41" spans="2:6">
       <c r="B41">
-        <f>LEFT(B11,2)*1</f>
+        <f t="shared" si="4"/>
         <v>55</v>
       </c>
       <c r="C41">
-        <f>F11/100</f>
+        <f t="shared" si="5"/>
         <v>0.26500000000000001</v>
       </c>
       <c r="E41" s="7">
@@ -3471,11 +3471,11 @@
     </row>
     <row r="42" spans="2:6">
       <c r="B42">
-        <f>LEFT(B12,2)*1</f>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="C42">
-        <f>F12/100</f>
+        <f t="shared" si="5"/>
         <v>0.29100000000000004</v>
       </c>
       <c r="E42" s="7">
@@ -3489,11 +3489,11 @@
     </row>
     <row r="43" spans="2:6">
       <c r="B43">
-        <f>LEFT(B13,2)*1</f>
+        <f t="shared" si="4"/>
         <v>65</v>
       </c>
       <c r="C43">
-        <f>F13/100</f>
+        <f t="shared" si="5"/>
         <v>0.34299999999999997</v>
       </c>
       <c r="E43" s="7">
@@ -3507,11 +3507,11 @@
     </row>
     <row r="44" spans="2:6">
       <c r="B44">
-        <f>LEFT(B14,2)*1</f>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="C44">
-        <f>F14/100</f>
+        <f t="shared" si="5"/>
         <v>0.43700000000000006</v>
       </c>
       <c r="E44" s="7">
@@ -3525,11 +3525,11 @@
     </row>
     <row r="45" spans="2:6">
       <c r="B45">
-        <f>LEFT(B15,2)*1</f>
+        <f t="shared" si="4"/>
         <v>75</v>
       </c>
       <c r="C45">
-        <f>F15/100</f>
+        <f t="shared" si="5"/>
         <v>0.47700000000000004</v>
       </c>
       <c r="E45" s="7">
@@ -3543,11 +3543,11 @@
     </row>
     <row r="46" spans="2:6">
       <c r="B46">
-        <f>LEFT(B16,2)*1</f>
+        <f t="shared" si="4"/>
         <v>80</v>
       </c>
       <c r="C46">
-        <f>F16/100</f>
+        <f t="shared" si="5"/>
         <v>0.46299999999999997</v>
       </c>
       <c r="E46" s="7">

</xml_diff>